<commit_message>
Added Article Author, Comment Author, Comment Target to CommentScrape
Added Article Title, Author, Date posted to ArticleScrape. No number of visitors added since I cannot recreate/find it.
</commit_message>
<xml_diff>
--- a/KinjaArticles.xlsx
+++ b/KinjaArticles.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,11 +14,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>Article Link</t>
   </si>
   <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Date Posted</t>
+  </si>
+  <si>
     <t>Num Comments</t>
   </si>
   <si>
@@ -37,7 +46,58 @@
     <t>http://itheedread.jezebel.com/1707231668</t>
   </si>
   <si>
+    <t>Only a Classless Douchebag Would Propose During Someone Else's Wedding</t>
+  </si>
+  <si>
+    <t>Mark Shrayber</t>
+  </si>
+  <si>
+    <t>5/27/15 3:15pm</t>
+  </si>
+  <si>
     <t xml:space="preserve"> A month ago, I was at my best friend’s wedding and joked to my partner about how funny it would be if we took a moment during the reception to propose to each other. We laughed and laughed and laughed. And then we checked to make sure that no one had been sent to kill us. Because no one even thinks about fucking up the bride’s special day without consequence.But there are people out there; people who are not like me and my partner and not like you. People who will do anything for attention. People who think that imposing themselves on someone else’s special day will somehow make the day more special for the others. People who believe that they have the right to do whatever they want because we live in America and if you want to get married there’s no more romantic place to ask than right before dessert during someone else’s wedding. These people are ill-mannered and ill-bred. These people are gigantic dicks. These people ruin weddings. No, really, they do.(Before you get angry because your sister totally said it was cool—she probably didn’t mean it, but we’ll set that aside—and you had discussed it beforehand, please let me make it clear that I am speaking about unplanned, unrehearsed and unwelcome proposals, not about a tearful moment everyone was enthusiastically a part of.)Earlier this week, a photo circulated on Reddit depicting a man proposing to his girlfriend in front of the bride and groom’s table at a wedding. While some believed that the bride looked happy, anyone who takes a look at her eyes can see that there is murder inside them. The motherfucking proposer even put down his goddamn Corona right in front of the bride (like her table was a fucking countertop?) before getting down on his knee to ask his intended to marry him in the middle of someone else’s party. Look at everything that is wrong in this picture:Those are not tears of happiness on the bride’s face, my friend. Those are tears of anguish. Those are tears that only a woman whose wedding has been derailed by an inconsiderate douche in a badly fitting shirt can cry. Those are tears that she will remember long after her wedding night. And when her friend calls her two months later, asking why they haven’t spoken since the wedding, the bride will remember only that moment when a day she’d planned for months was squashed by the very people she thought to be closest to her (not her horrible parents, not her racist uncle, but her.best.friend.) and flatly say, “I’ve just been really busy,” before making an excuse to get off the phone quickly and search Google for “how to block a number on Sprint.”But just in case this picture isn’t convincing enough (and it should be, assuming you’re not a monster), I have a whole list of reasons why you should never ever propose during someone else’s reception. (I am of the belief that you shouldn’t even ask to do so because people will feel guilty and let you, but that’s between you and them. This is just about the surprise proposal.)It’s not your day.I understand how some people may not get this and also think that brides and grooms would want to share their special day with everyone they’ve invited, but make no mistake: It’s about them sharing their happiness with you, not about you sharing your happiness with them. You wouldn’t like it if someone strolled into your birthday party and demanded that “Happy Birthday” be sung to them, so others probably won’t like it if you decide that their special day is now just a special day in general. And think about this: You get like 80 birthdays so if one is annoying, whatever. But how many weddings does the average person have? Three? No, those are too precious to be mucked up by your tearful proposal.A good time to propose is after a wedding, not during one. And if you propose right before a wedding, I’d say keep it on the DL—but, you know, do you as long as you’re not doing it in the middle of a wedding, you know?Let me give you an example that has nothing to do with weddings but will make sense as an analogy:It took me forever to graduate college, so when I finally did I planned a graduation dinner at The Olive Garden, invited everyone I loved and went down there and waited in line for two hours because, as you know, the O.G does not accept reservations.Right before my party, my mom, who was not paying for this or anything, just an invited guest, called me up and told me that she was inviting my brother’s friends and that this was going to be a joint party for the both my brother and me because he was transferring to a school out of town. Girl, what? Yes. She brought my brother’s friends, and she gave a toast saying how proud she was of me but also let’s talk about my brother, since suddenly this was his party, too. Now imagine if that had happened to you. Is it petty to feel shitty about something like that? Maybe. But someone just took away an important moment and no matter how chill you are, your initial reaction will likely be anger and disgust.So just remember that: It’s not your day. You can have your own day. Just not today. Not in the middle of someone else’s reception.Weddings are expensive.That’s why people want them to be perfect! Someone is paying $4,000 for centerpieces, they want to make sure that everything is going according to plan. That means the toasts better happen when they’re meant to, that the dance mix will not be made up of audience requests (because how many times can you listen to “Like a Virgin” in one night?) and that the spotlight will be on the happy couple the entire night, even if they’re doing dopey shit like a literal interpretive dance to a country song. Yes, some things will invariably go wrong (the power went out during the dancing at the last wedding I went to), but those things should not be due to the wedding guests deliberately trying to steal the spotlight of someone else’s expensive one-time affair, regardless of whether it cost $200 or $20,000 to put on. (Also: don’t ask about the cost of a wedding, I recently learned that that’s tacky.)It is not truly spontaneous.You and I both know that if you get up there and say, “I wasn’t planning on doing this but seeing soooo much love out there tonight has made me think about my own relationship,” you are a liar. You have thought this through every step of the way. You could have stopped yourself at any time. It’s even worse if you have a ring for this “spontaneous” moment. You weren’t planning on doing this? Then how come you got a big sparkly-ass diamond in your pocket? It just fell in there? Is there a positive pregnancy test in there, too? No, don’t tell me! Wait for someone’s baby shower!My point is that best-case scenario your proposal is a premeditated attack, worst-case it really is a spontaneous decision which means you haven’t thought very much about it and it actually doesn’t mean anything which is even more upsetting and useless. Just eat your Beef Wellington and vinegar salad and propose somewhere else.You’re doing it for attention.Yes, you are! Even if you cleared it with the bride and groom first! There are probably going to be people at this wedding who have no idea who you are and didn’t need to be trapped in this awkward moment. If you really must propose when your entire family is present, at least do it at the brunch after the wedding when everyone is hungover and the happy couple just want everyone fucking gone so they can go home and take a nap. (It’s still a tacky thing to do, but it’s more forgivable? I don’t know.)You’re making it all about you.After the proposal, the evening will belong to you. The highlight won’t be the bride and groom’s first dance or the cake. It will forever be known as the wedding that was crashed by your proposal. That’s how it’ll be remembered. At my wedding I plan on descending from the ceiling in a sparkle suit (Parisian carnival theme wedding, here I come!) while slowly cartwheeling through the air. That’s what people should remember, not the fact that someone proposed during the toasts in my beautiful Cirque Du Soleil-inspired reception.People love something new and exciting. If you propose during a wedding, guess what: That’s you! The married couple is now old hat. They’ve been married for like an hour already. BORING! But you! You just got engaged! You’re shiny and new and have so much to plan and everyone wants to talk to you and congratulate you and no matter what you believe there really is a finite amount of attention in the world and it is not going to the people for whom this event is being thrown right now. And that goes double for people who sent out really special invites, save-the-dates that were magnets, or have an Instagram hashtag for pictures.And to people who say, “Well, my wedding isn’t about, like, attention,” I say bullshit. It may not be about garnering attention for yourself the entire time, but it most certainly is about about your day and your love. That is about you. Don’t tell me you wouldn’t be a tiny bit peeved if an overwhelming amount of the focus went somewhere else.There are, of course, other ways for you, as a guest, to make the day special and show off to others how cool you are without actually disrupting the day that wasn’t about you to begin with. The best way is to be an excellent or unique dancer who will literally throw themselves on the floor during “Blank Space” (me) or remove their shirt during part of the dancing portion (also me). You could also do your best if you’re invited to do a reading and, most importantly, you can kill it during your toast. Just as long as your toast is about the happy couple and not how awesome you are. (You are awesome. Just less awesome than the couple for today.)One more thing you can do to make the wedding as enjoyable as possible without being disruptive: Eat until you burst and then also eat as many wedding favors as possible. At a recent wedding I wasn’t invited to do a reading or give a toast and had to do something to curb my undying thirst for attention, so I ate about 25 cookies with my friend’s name on them. That filled me right up until my next therapy session. Try it, you’ll like it.Update: The bride pictured has informed the public that the proposal was planned and approved. According to her, everyone but the proposee knew it was coming (which comes with its own set of problems that I didn’t even get to) and everyone is really happy (mmm...) about everything. My argument has not changed: Proposing in the middle of someone’s wedding, unplanned, is a douchebag move.</t>
+  </si>
+  <si>
+    <t>http://www.avclub.com/1798447330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Day After traumatized a generation with the horrors of nuclear war </t>
+  </si>
+  <si>
+    <t>Sean O'Neal</t>
+  </si>
+  <si>
+    <t>8/28/17 5:42pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In Apocalypse Then, we revisit movies that depict the onset of nuclear war and the immediate aftermath of annihilation. You know—for fun.  As a plot device, the apocalypse is as old as fiction itself. Old enough to appear in the epic poems passed around Mesopotamia, where tales of great, world-destroying floods were shrugged off as just a bunch of liberal hand-wringing. Old enough to inspire countless myths, murals, and Kirk Cameron movies—an entire genre where humans perishing cataclysmically remains the guaranteed showstopper. But while the “apocalypse movie” has become something of an an annual tradition, with godlike filmmakers destroying mankind with all manner of imaginative plagues, environmental disasters, and alien invasions, films about nuclear apocalypse, specifically, arguably remain the most fascinating, precisely for how unimaginative it is. There’s nothing supernatural about nuclear war; here, the fate of the world is entirely within our clumsy, spiteful human hands. What could be more horrifying?From the very first atomic bomb tests, to the horrors of Hiroshima and Nagasaki, to the gallows paranoia of the Cold War, our movies have long been filled with nuclear fallout, spawning ridiculous monsters and maudlin messages alike in its radioactive wake. The psychological appeal of this is obvious: It allows us to confront our own terrible powers, to ponder the flimsy thread that civilization dangles on, and to peer into the dark abyss of human nature, all with plenty of rip-roaring explosions. And it allows us to pretend as though we are taking corrective measures to prevent doing ourselves in, just by watching a movie about it. But it also allows us to absolve ourselves of caring too much about anything, because hey, we’re all probably just going to end up dying in a smoking crater anyway.In this column, we’ll be looking at some of the many depictions of our impending nuclear doom cinema has served up over the years, to see what they can tell us about the times they were released in—and can still tell us about ourselves. (Notice I said “impending”: We won’t be examining post-apocalyptic movies here, which is an entire genre unto itself.) We begin with a film that’s gotten a surprising amount of play again recently as we—unbelievably, unthinkably—are all forced to bone up again on what might happen if some tough-talking madman gets us all nuked:The Day After (1983)ABC’s TV movie The Day After runs a mere two hours—edited, clumsily at times, down from a sprawling four. But as a cultural touchstone, whose reputation for leaving an entire generation traumatized and jaded, it’s endured far longer. Modern audiences were reminded of that last year in an episode of The Americans, in which our beloved blithely neck-snapping, organ-liquefying Soviet sleeper agents are briefly cowed into morally questioning quietude after they gather to watch it in their living room. The way the show treats it as an epochal, moon landing-like event isn’t really an exaggeration: More than 100 million people really did drop everything to watch it on November 20, 1983, with many sitting in stunned horror and having their own existential conversations afterward about how we were all basically screwed.Those talks had been going on for weeks, actually, along with alarmist debate over what kind of messages The Day After would send, of the political upheaval it would cause, of the havoc it would wreak among panicked viewers, of the permanent damage it might cause to all the precious children who watched it. ABC even took the rare step of issuing a special “Viewer’s Guide” that provided a series of discussion questions and thought “exercises” for both before and after watching, then set up 1-800 hotlines for anyone who needed counseling. And while most of that anticipated, widespread trauma failed to materialize—though you’ll definitely find people who will attest that, yeah, seeing this movie at a tender age fucked them up pretty good—there was a definite ripple effect, both on nuclear policy and American attitudes toward it. Though it’s hardly the scariest or even the most compellingly told, The Day After may well be the most impactful film ever made about the devastation of nuclear war. It’s crazy to think it aired in a time slot normally reserved for Hardcastle &amp; McCormick. Personally speaking, I didn’t catch The Day After in its original run; I was 5 years old at the time, and while my parents weirdly had no problem letting me glimpse the occasional breast on an HBO broadcast of Valley Girl, they wisely drew the line at exposing mommy’s precious boy to global annihilation. Still, even decades removed from the furor, and after years of watching our fair cities blown to fake smithereens, it’s amazing how The Day After still retains a lot of its impact, even if you just watch it on YouTube (which you can do right now). Much of its effectiveness can be attributed to the fact that it’s so surprisingly, unrepentantly bleak—by any contemporary standard. This isn’t the kind of movie where Armageddon is just a teachable moment, prompting characters to gaze into the scorched middle distance and wonder aloud about man’s inhumanity to man. I mean, there’s a little bit of that, sure. But the reason The Day After probably left so many shaken is that it does far more showing than telling, letting its piles of charred corpses and slowly accumulating radiation blisters speak more than teary monologues ever could.Its morbidity, even at the expense of being moving, can largely be attributed to director Nicholas Meyer, who fought at every step for his to be a brutally straightforward depiction—something he undertook as a “civic responsibility,” as he told The Washington Post in ’83. Meyer inherited the project, which was dreamed up by ABC executive Brandon Stoddard, right when he could have just been riding high after Star Trek II: The Wrath Of Khan, making more escapist blockbusters about far more charismatic destructors. Instead, he took on a deeply, nauseatingly well-researched and graphic script from Edward Hume, then approached the project as a “public service announcement,” not entertainment. “From my perspective it isn’t a very good movie,” Meyer said in a recent interview. “And more than that, it was not intended to be a very good movie.”Meyer’s right: The Day After isn’t a very good movie, at least not in the usual sense. It’s pretty sluggish for its entire first hour, poking around the farmlands of Lawrence, Kansas while introducing its various milk-fed, salt-of-the-soon-to-be-salted-earth characters. After sitting through their various standard family drama subplots for an hour, you kind of can’t help but wonder when they’re gonna get to the genocidal fireworks factory. And after the bombs finally do drop, its second half suffers from that aforementioned clumsy editing, as characters disappear for long stretches, get desultorily dispatched off-screen, or just end up abandoned altogether. Time also hasn’t been particularly kind to its special effects, which, even by 1983 standards, have a distinctly painted-on feel. The exceptions are the tangibly scarred downtown streets and blown-out buildings, which were smashed up by a production that descended on Lawrence like its own purgative fire. Meyer then reportedly paid hundreds of locals $75 a head to shave them bald and plaster on latex scars until they resembled sickly, molting chickens, which the townspeople eagerly took on as a fun little brush with movie magic.But in the sense that movies should provoke some sort of emotional reaction, The Day After is unusually effective—largely due to that reliance on using real people. Meyer actually didn’t want to use any famous actors, concerned it would only take viewers out of it and reassure them that this was all just some Hollywood fantasy. But after the network said it needed someone it could sell to foreign markets, in stepped Jason Robards—who was coming off Oscar-recognized turns for All The President’s Men, Julia, and Melvin And Howard—to play the kindly Dr. Oakes, who somehow survives the blast by ducking down in the front seat of his car (they don’t build ’em like that anymore), then staggers 10 miles back to the University Of Kansas to lead triage efforts for the survivors. The weight of the world, as always, rests on Robards’ eyebrows here, but even his performance feels subsumed by the mass of shattered, anonymous faces that surround him.Of course, time has lessened this effect as well: The Day After is full of people you’d recognize now—and even a few you would have back in ’83. JoBeth Williams, who plays Nurse Bauer, was in the middle of a hot run that stretched from Stir Crazy to Poltergeist to The Big Chill. As the worldly Professor Huxley, John Lithgow was fresh off his Oscar-nominated breakout in The World According To Garp—which makes his relatively minor role seem like a squandered opportunity. There’s also Animal House’s Stephen Furst as one of Lithgow’s students, and a brink-of-stardom Amy Madigan as a pregnant woman who’s understandably conflicted about bringing a child into the newly destroyed world. Most distractingly, there is Steve Guttenberg, in the fulcrum between Diner and Police Academy, playing a college student whose Midwestern twang flits in and out—and who’s first introduced in his tighty-whities. And finally, there is Northern Exposure’s John Cullum as the patriarch of a family riding out the blast in its cellar. At the time, Cullum was more of a Broadway star, but was nevertheless such a familiar, comforting presence, it fell to him to warn ABC viewers of the “unusually disturbing” images they were about to see—right after the ABC announcer explained why they wouldn’t be getting Hardcastle &amp; McCormick that night. (Would Hardcastle be able to take down that gang of car thieves? Would we live long enough to see it?!)Even in their relatively primitive state—even when surrounded by the intermittent amusement of the Gute, strutting around in ’80s jeans tucked up to his armpits—those images are still plenty jarring. The attack sequence in particular remains riveting, a series of clever crosscuts between government missile test footage and scenes of all those average Midwesterners, watching ominous vapor trails appear over gazebos in the park, before being flash-frozen in the blast. Though significantly toned down from the script’s original plans to show skin and eyes melting, or faces blasted from skulls, it’s arguably even more effective in its restraint. Maybe it’s the sentimentality brought on by new parenthood, but I haven’t been able to shake the image of a mother holding her baby as they’re transformed into glowing X-ray skeletons, evaporated in an instant.In the aftermath that takes up its back hour, The Day After becomes a genuine horror film as its characters begin to succumb to radiation poisoning, their hair and teeth falling out as they shamble through scorched fields strewn with bloated animal corpses and dead family dogs, swarming with flies. Befitting the deathly pallor, Meyer imbues these scenes with classically gothic imagery: a bell struck by an unseen hand wielding a brick summons survivors from the crypts of their shelters; a lighthearted conversation between Robards and Williams is interrupted by a bandaged woman sitting up into frame and shrieking; a preacher gives a sermon inside the crater of a church, a burned crucifix dangling behind him; a young woman sitting in the pews begins suddenly bleeding from between her legs into her white dress. A bit heavy-handed, maybe—but then, there’s nothing subtle about apocalypse. And as the end title card reminds us, even this grisly depiction is still “in all likelihood, less severe than the destruction that would actually occur,” not to mention wholly more cinematic.Just by attempting to show that devastation, its critics preemptively argued, The Day After was making a political statement. Conservative commentators like William F. Buckley decried the film for being anti-deterrence; “No Nukes” protesters embraced it as the same, holding candlelight vigils and rallies around its airing. For his part, Meyer rebuked both sides: “I don’t want a conservative backlash saying ‘Oh, this is just the Jews in Hollywood, this is just liberals in Hollywood, mounting their soapbox,’” he told the Post (a statement that still feels sadly contemporary). He resisted the idea that The Day After had any political message beyond, as he told an Australian news station, “that nuclear war is bad for you, and that if a nuclear bomb goes off it’s going to ruin your entire day.” As such, the film deliberately obscures who shot first. “What does it matter?” asks one survivor, a college student seen earlier confidently spouting off about geopolitics. Lithgow’s professor responds by morosely quoting Einstein: “I know not with what weapons World War III will be fought, but World War IV will be fought with sticks and stones.” Who cares about politics when we’re all sifting through the rubble? Nevertheless, it raised enough hackles to prompt a tense special edition of Nightline that immediately followed, with nuclear freeze advocates like Carl Sagan squaring off against Buckley, Henry Kissinger, and Robert McNamara. (Watching that debate now, it’s dismaying how relevant the discussion feels still—not to mention how much more respectfully it’s conducted than any given TV discussion today.) And the movie famously influenced Ronald Reagan, who wrote in his diary that watching it “left me greatly depressed.” After signing a 1987 nuclear treaty with the Soviet Union’s Mikhael Gorbachev, Reagan sent a telegram to Meyer, saying, “Don’t think your movie didn’t have any part of this, because it did.”Reagan is never mentioned by name in The Day After, though he did make a sort-of-cameo  in the form of an actor doing a passable impression of his halting wheeze in a radio broadcast, aimed at reassuring survivors that there had been “no surrender, no retreat from the principles of liberty and democracy”—ironically juxtaposed with stunned, soot-covered mole people who could really give a shit. After this scene was denounced as tantamount to a political attack, the actor was overdubbed with another, more generically patrician voice for later versions.Like the scene where Cullum’s farmer is given the laughable, FEMA-sourced advice to just “scrape off” his irradiated topsoil, it’s in moments like these that The Day After’s actual—and again, sadly relevant—message makes itself known: Should we be  hit with nuclear missiles, no one will really know what to do about it. Hell, if it happens sooner rather than later, we won’t even have the cold comfort of a president who can offer up some eloquently empty words. That’s why, watching it today, the most chilling aspect of The Day After isn’t the bombs, or their grisly aftermath. It’s all the scenes leading up to it, as people go about their lives with snatches of news broadcasts overheard—and ignored—in the background reporting on some tense, but relatively minute skirmish in Berlin. Even Lithgow’s politically informed, astutely cynical intellectual laughs off the idea of escalation, saying he has symphony tickets. The soldiers stationed around Lawrence’s missile silo joke about nuclear war infringing on their weekend fishing plans. Robards’ wife sees an alarmist special bulletin, moans, and says she just wants to go to bed. Even as the world teeters on the edge, Robards pauses to ask, to no one in particular, “Do you understand any of this?” Throughout, the threat of cataclysmic war remains a distant, inscrutable, headache-inducing hum, something to be switched off as soon as it becomes too complicated to follow. If it were made today, you could easily cut in shots of people paging listlessly through Twitter.“We knew this could happen for 40 years. Nobody was interested,” Madigan says during one of the film’s more on-the nose moments. Yeah, well, it’s been another 34 since then, and people aren’t exactly getting worked up about it today either, even as nuclear brinkmanship has now expanded to include some far more unpredictable new players, and the codes put in the hands of impulsive zealots who, unlike Reagan, don’t have the capacity to reflect somberly on much of anything. In the meantime, we’ve only become even more numbed to nuclear war by decades of way better-looking mushroom clouds dotting our TV and movie screens—just one more obstacle for a superhero to come and throw CGI at. If The Day After has anything to warn us about today, it’s that we’re still woefully unprepared for something we’ve been worrying about—and shrugging off—for as long as we can remember.</t>
+  </si>
+  <si>
+    <t>http://www.avclub.com/1798505721</t>
+  </si>
+  <si>
+    <t>This season of Game Of Thrones was illogical, dumb, and fun as hell</t>
+  </si>
+  <si>
+    <t>8/28/17 2:00pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Photo: HBONote: This article touches on plot points from Game Of Thrones’ seventh season.This season of Game Of Thrones was a fast-paced, wildly fun ride filled with huge battle sequences, long-awaited reunions, thrilling team-ups, and some of the most memorable deaths in the series’ history. This season of Game Of Thrones was a knowingly rushed, ludicrously implausible bit of fan service, filled with improbable character alliances that seemed like they were lifted from some multiplayer video game, romances that felt like direct pandering to “shippers,” and some of the least surprising ends for the most relatively disposable characters left in a show that’s rapidly running out of major players to kill. These statements sum up the general sentiments on either side of the drama’s polarizing seventh season—and I agree with both of them. This season was breakneck, sloppy, and occasionally downright stupid. It was also a lot of fun.There are few series in TV history that have invited the kind of granular analysis that Game Of Thrones gets on an hourly basis. (Those of us here in the crumbling online media world will surely have to shutter our doors the week after its final episode airs.) In all that talk, “Was it fun?” tends to get the shaft. Perhaps it’s the need to overcompensate for what sounds, superficially, like a very silly story, but Game Of Thrones has always been held to a very serious, surprisingly rigid internal logic for a show about dragon-riding queens fighting ice zombies, all while surrounded by imps, sorcerers, and the largest cast of eunuchs ever assembled. Most of that solemnity can, of course, be attributed to author George R.R. Martin, whose commitment to realistic character development and cautious buildup—to documenting the many gradual changes that provide more depth to a sudden stabbing—is rare in fantasy fiction. As such, it’s mirrored in the many fans who will complain on Martin’s behalf whenever that stuff is sped through or omitted completely. In an interview with io9 a few years back, Martin explained his approach while discussing the reader reaction to A Feast For Crows:I get complaints sometimes that nothing happens—but they’re defining “nothing,” I think, differently than I am. I don’t think it all has to be battles and sword fights and assassinations. Character development and [people] changing is good, and there are some tough things in there that I think a lot of writers skip over. I’m glad I didn’t skip over these things… I guess there is an element of fantasy readers that don’t want to see that. I find that fascinating. Seeing someone like Dany actually trying to deal with the vestments of being a queen and [dealing with] factions and guilds and the economy. They burnt all the fields [in Meereen]. They’ve got nothing to import anymore. They’re not getting any money. I find this stuff interesting. And fortunately, enough of my readers who love the books do as well.I guess I’m one of those fascinatingly bad fantasy readers—actually, I know I am—because guild negotiations and the ins and outs of the grain trade are exactly the sort of stuff I usually find stultifying about the genre, and it’s why I’ve never been remotely interested in playing something like, say, Settlers Of Catan. I don’t begrudge anyone else’s fascination with the details, just like I don’t find anything wrong with indulging in speculation over how and where, exactly, the White Walkers could best circumvent the Wall. For some, these are the pursuits that enrich the story and deepen their connection. On my end, I was perfectly happy that the White Walkers just ended up taking a big fucking ice dragon to it. It was a big, obvious, ham-fisted narrative decision that was completely lacking in subtlety and, most likely, proper dragon science. But it made for great television.Despite also understanding the dissent, I have likewise enjoyed the fact that this season, characters appeared to have magically unlocked warp zones that allowed them to pop up in distant lands over the course of an episode; that Jon Snow, through sheer screenwriter contrivance, conveniently managed to assemble an Avengers dream team out of all the series’ most badass secondaries; that this team then went on a totally badass, yet laughably ill-thought-out suicide mission to swing some flaming swords at a vast undead army; that they were only rescued by Daenerys swooping in to save them, atop a dragon that she could have easily swept over a field of wights her damn self without sacrificing anyone. I get that, to some people, these things represent utter betrayals of characters who have in the past been shown to be relentlessly meticulous tacticians, or that they don’t even appear to be born from the same source material, which has always been so methodical about its plotting and geography. But, bad fantasy fan that I am, I’ve found this season’s reckless disregard of the specifics to have invigorated a show that has, in my opinion, occasionally gotten way too bogged down in them.This opinion, I should say, isn’t a popular one among my co-workers. I’ve already been told today that all this has just ended up making Game Of Thrones a far more conventional show—that it’s done away with the fascinating gray area where so many of its characters used to dwell, reducing them to clearly delineated “good guys” and “bad guys” in this looming war between living and dead. I’ve also been told that it’s completely deflated the show of any tension and robbed it of its capacity to surprise; that there are no genuine emotional stakes anymore; that it’s lost the intrigue that once made it unique. I get what they’re saying, and I respect it. Generally, I’m not a big “It’s just a TV show, so turn off your brain!” guy. But I still find myself not particularly caring.Our disagreement, I think, can be attributed to their appreciating the series from a novelistic perspective—as a worthy extension of Martin’s carefully plotted, still-unfinished saga—versus my own approach to the show, which is looking for nothing more than pure, episode-by-episode enjoyment. Game Of Thrones spent its first five seasons carefully balancing the two, all dictated by the meted-out sudden twists mapped out in Martin’s books. But from my perspective as a spoiled-for-choice TV viewer and bad fantasy reader—and as someone who finds endless conversations about honor and power and what it means to rule a little tedious—I guess I prefer all those battles, the sword fights, and the assassinations that allowed Martin the latitude to get back to his imaginary economics (or those endless descriptions of someone’s dinner).In that sense, Game Of Thrones’ seventh season was a ramshackle, occasionally dumb, frequently fan-servicing, kinda shallow mess, and I enjoyed it all very much. Compared to previous seasons, it was also disproportionately rich with scenes that, when looking back on the show’s complete run years from now, I will vividly recall: Arya’s revenge on Walder Frey; Euron’s over-the-top attack on Yara’s fleet; (especially) Cersei’s traumatic punishment of Ellaria Sand; Olenna Tyrell turning her own death into a cool kiss-off; Sam finding the most obvious, grisliest possible cure for Jorah’s grayscale; the dragons laying waste to the Lannister army; the finale’s all-hands conference for its major characters, etc. etc. The fact that all of these memorable moments were crammed into a mere seven episodes is admittedly ludicrous. It also made for an exceptionally entertaining couple of months.My suspicion is that the eighth and final season will take a slightly steadier hand, and—by the end, at least—it will have returned to the more deliberate pacing and thoughtful rumination that once defined the show. But that will have been made possible by this season, with its mad, implausible, logic-defying race to get all the characters positioned just so, and its utter disregard at times for all the “nothing” that used to happen in between. And because of it, I find myself anticipating that final run even more.</t>
+  </si>
+  <si>
+    <t>http://www.avclub.com/1798517837</t>
+  </si>
+  <si>
+    <t>Evangeline Lilly celebrates Jack Kirby's birthday with Ant-Man And The Wasp pic</t>
+  </si>
+  <si>
+    <t>Sam Barsanti</t>
+  </si>
+  <si>
+    <t>8/28/17 6:00pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (Photo: Getty Images, Jason Merritt)Today would’ve been the 100th birthday of legendary comic book creator Jack Kirby, and while he didn’t live to see so many of the creations that publishers refused to pay him for hit the big screen, some of the people involved in making movies about his creations are still setting time aside today to honor his work. Ant-Man And The Wasp star Evangline Lilly is one such person, and she—or at least Marvel Studios, through her Twitter account—decided to honor Kirby’s legacy by revealing a new photo of what Hope Van Dyne will look like in the Ant-Man sequel once she suits up.The outfit looks a bit more muted than most of The Wasp’s costumes in the comics, as is to be expected in a live-action movie, but it does look fairly faithful otherwise—although her helmet and wings aren’t pictured, since Marvel has to hold something back for the trailers.</t>
   </si>
 </sst>
 </file>
@@ -411,12 +471,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +484,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,30 +503,138 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="n">
         <v>2015</v>
       </c>
-      <c r="C2" t="n">
+      <c r="F2" t="n">
         <v>119</v>
       </c>
-      <c r="D2" t="n">
+      <c r="G2" t="n">
         <v>1890</v>
       </c>
-      <c r="E2" t="n">
+      <c r="H2" t="n">
         <v>10535</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="n">
+        <v>364</v>
+      </c>
+      <c r="F3" t="n">
+        <v>16</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2706</v>
+      </c>
+      <c r="H3" t="n">
+        <v>16741</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="n">
+        <v>289</v>
+      </c>
+      <c r="F4" t="n">
+        <v>9</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1325</v>
+      </c>
+      <c r="H4" t="n">
+        <v>8068</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="n">
+        <v>88</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" t="n">
+        <v>154</v>
+      </c>
+      <c r="H5" t="n">
+        <v>889</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>